<commit_message>
Markup TB und MF
Markup TB und MF, Ergänzungen Orts- und Personenregister
</commit_message>
<xml_diff>
--- a/docs/Baernreither_Ortsregister_2023.xlsx
+++ b/docs/Baernreither_Ortsregister_2023.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="282">
   <si>
     <t>Biala</t>
   </si>
@@ -848,6 +848,33 @@
   </si>
   <si>
     <t>https://www.geonames.org/3337514/istria.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/2635167/united-kingdom-of-great-britain-and-northern-ireland.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/3054667/buda.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.geonames.org/6559171/muenchen-landeshauptstadt.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/3067696/prague.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/3068160/pilsen.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/11748058/silesian-metropolis.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/3061822/zatec.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/3071024/marianske-lazne.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/3068119/podborany.html</t>
   </si>
 </sst>
 </file>
@@ -1357,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="134" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="134" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1707,7 +1734,9 @@
       <c r="D22" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="8"/>
+      <c r="E22" s="8" t="s">
+        <v>273</v>
+      </c>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2073,7 +2102,9 @@
       <c r="D47" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E47" s="4"/>
+      <c r="E47" s="4" t="s">
+        <v>280</v>
+      </c>
       <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2115,7 +2146,9 @@
       <c r="D50" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E50" s="4"/>
+      <c r="E50" s="4" t="s">
+        <v>275</v>
+      </c>
       <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2193,7 +2226,9 @@
       <c r="D56" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="E56" s="4"/>
+      <c r="E56" s="4" t="s">
+        <v>274</v>
+      </c>
       <c r="F56" s="4"/>
     </row>
     <row r="57" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2259,7 +2294,9 @@
       <c r="D61" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="E61" s="4"/>
+      <c r="E61" s="4" t="s">
+        <v>277</v>
+      </c>
       <c r="F61" s="4"/>
     </row>
     <row r="62" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2273,7 +2310,9 @@
       <c r="D62" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E62" s="4"/>
+      <c r="E62" s="4" t="s">
+        <v>281</v>
+      </c>
       <c r="F62" s="4"/>
     </row>
     <row r="63" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2313,7 +2352,9 @@
       <c r="D65" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E65" s="4"/>
+      <c r="E65" s="4" t="s">
+        <v>276</v>
+      </c>
       <c r="F65" s="4"/>
     </row>
     <row r="66" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2393,7 +2434,9 @@
       <c r="D71" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E71" s="4"/>
+      <c r="E71" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="F71" s="4"/>
     </row>
     <row r="72" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2419,7 +2462,9 @@
       <c r="D73" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E73" s="4"/>
+      <c r="E73" s="4" t="s">
+        <v>278</v>
+      </c>
       <c r="F73" s="4"/>
     </row>
     <row r="74" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Markp MF Personen und Orte
</commit_message>
<xml_diff>
--- a/docs/Baernreither_Ortsregister_2023.xlsx
+++ b/docs/Baernreither_Ortsregister_2023.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="285">
   <si>
     <t>Biala</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Cilli</t>
   </si>
   <si>
-    <t>Königsberg</t>
-  </si>
-  <si>
     <t>Polnisch-Ostrau</t>
   </si>
   <si>
@@ -277,9 +274,6 @@
     <t>Sangerberg</t>
   </si>
   <si>
-    <t>Königswart</t>
-  </si>
-  <si>
     <t>Eger</t>
   </si>
   <si>
@@ -790,9 +784,6 @@
     <t>3 Königsberg in Tschechien - nachsehen, welches</t>
   </si>
   <si>
-    <t>2 Königswart in Tschechien - nachsehen, welches</t>
-  </si>
-  <si>
     <t>https://www.geonames.org/3197905/kokra.html</t>
   </si>
   <si>
@@ -875,13 +866,31 @@
   </si>
   <si>
     <t>https://www.geonames.org/3068119/podborany.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/2988507/paris.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/3067688/prameny.html</t>
+  </si>
+  <si>
+    <t>Koenigswart</t>
+  </si>
+  <si>
+    <t>Koenigsberg</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/3072265/lazne-kynzvart.html</t>
+  </si>
+  <si>
+    <t>CA: habe das in der Nähe von Marienbad gewählt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -907,6 +916,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -951,7 +967,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -989,6 +1005,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1384,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="134" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="134" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1399,10 +1418,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
@@ -1414,72 +1433,72 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
@@ -1488,32 +1507,32 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1523,65 +1542,65 @@
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F12" s="4"/>
     </row>
@@ -1592,305 +1611,305 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="13" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="4"/>
@@ -1898,111 +1917,113 @@
     <row r="34" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="D35" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>13</v>
+        <v>282</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>82</v>
+        <v>281</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4" t="s">
-        <v>253</v>
+        <v>122</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -2010,39 +2031,39 @@
     <row r="41" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -2050,89 +2071,89 @@
     <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -2140,41 +2161,41 @@
     <row r="50" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
     <row r="52" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
@@ -2182,11 +2203,11 @@
     <row r="53" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -2194,11 +2215,11 @@
     <row r="54" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -2206,37 +2227,37 @@
     <row r="55" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
     </row>
     <row r="56" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F56" s="4"/>
     </row>
     <row r="57" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -2245,14 +2266,14 @@
     </row>
     <row r="58" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -2260,71 +2281,71 @@
     <row r="59" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
     </row>
     <row r="60" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
     </row>
     <row r="61" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F61" s="4"/>
     </row>
     <row r="62" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F62" s="4"/>
     </row>
     <row r="63" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -2332,13 +2353,15 @@
     <row r="64" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="B64" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E64" s="4"/>
+        <v>160</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="F64" s="4"/>
     </row>
     <row r="65" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2350,63 +2373,63 @@
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F65" s="4"/>
     </row>
     <row r="66" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
       <c r="B66" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
     </row>
     <row r="67" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
     </row>
     <row r="68" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F68" s="4"/>
     </row>
     <row r="69" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="B69" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
@@ -2414,43 +2437,45 @@
     <row r="70" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
     </row>
     <row r="71" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F71" s="4"/>
     </row>
     <row r="72" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E72" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>280</v>
+      </c>
       <c r="F72" s="4"/>
     </row>
     <row r="73" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -2460,21 +2485,21 @@
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F73" s="4"/>
     </row>
     <row r="74" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="B74" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
@@ -2482,71 +2507,71 @@
     <row r="75" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
       <c r="B75" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
     </row>
     <row r="76" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F76" s="4"/>
     </row>
     <row r="77" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
     </row>
     <row r="78" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
     </row>
     <row r="79" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C79" s="4"/>
       <c r="D79" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
@@ -2554,67 +2579,67 @@
     <row r="80" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
       <c r="B80" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
     </row>
     <row r="81" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F81" s="4"/>
     </row>
     <row r="82" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A82" s="4"/>
       <c r="B82" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C82" s="4"/>
       <c r="D82" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
     </row>
     <row r="83" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
     </row>
     <row r="84" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="6"/>
@@ -2622,27 +2647,27 @@
     <row r="85" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
       <c r="B85" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C85" s="4"/>
       <c r="D85" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
     </row>
     <row r="86" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B86" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D86" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D86" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="E86" s="6"/>
       <c r="F86" s="4"/>
@@ -2654,21 +2679,21 @@
       </c>
       <c r="C87" s="4"/>
       <c r="D87" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
     </row>
     <row r="88" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C88" s="4"/>
       <c r="D88" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
@@ -2687,28 +2712,28 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E90" s="7"/>
       <c r="F90" s="4"/>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E91" s="7"/>
       <c r="F91" s="4"/>

</xml_diff>

<commit_message>
Markup TB 7 und MF 6-1 und Ergänzungen Ortsregister und OrgNames
</commit_message>
<xml_diff>
--- a/docs/Baernreither_Ortsregister_2023.xlsx
+++ b/docs/Baernreither_Ortsregister_2023.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="310">
   <si>
     <t>Biala</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Cilli</t>
   </si>
   <si>
-    <t>Polnisch-Ostrau</t>
-  </si>
-  <si>
     <t>Agram</t>
   </si>
   <si>
@@ -106,18 +103,12 @@
     <t>Triest</t>
   </si>
   <si>
-    <t>Görz</t>
-  </si>
-  <si>
     <t>Tirol</t>
   </si>
   <si>
     <t>Floridsdorf</t>
   </si>
   <si>
-    <t>Brüx</t>
-  </si>
-  <si>
     <t>Steiermark</t>
   </si>
   <si>
@@ -145,9 +136,6 @@
     <t>Ischl</t>
   </si>
   <si>
-    <t>Rakos-Palota</t>
-  </si>
-  <si>
     <t>Neupest</t>
   </si>
   <si>
@@ -769,9 +757,6 @@
     <t>https://www.geonames.org/3197986/knin.html</t>
   </si>
   <si>
-    <t>3 Königsberg in Tschechien - nachsehen, welches</t>
-  </si>
-  <si>
     <t>https://www.geonames.org/3197905/kokra.html</t>
   </si>
   <si>
@@ -926,6 +911,54 @@
   </si>
   <si>
     <t>StarnbergerSee</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/2017370/russian-federation.html</t>
+  </si>
+  <si>
+    <t>RakosPalota</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/3175395/italian-republic.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/3165241/provincia-autonoma-di-trento.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/6539916/rovereto.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/3165185/trieste.html</t>
+  </si>
+  <si>
+    <t>Goerz</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/11920184/opava.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/7532301/cieszyn.html</t>
+  </si>
+  <si>
+    <t>Bruex</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/11921844/kynsperk-nad-ohri.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/11921098/ostrava.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/11055010/zadar.html</t>
+  </si>
+  <si>
+    <t>Amerika</t>
+  </si>
+  <si>
+    <t>Vereinigte Staaten von Amerika</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/6252001/united-states.html</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1098,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1125,9 +1157,10 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1143,14 +1176,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:F91" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:F92" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
   <tableColumns count="6">
-    <tableColumn id="5" name="aktuelle Schreibung" dataDxfId="5"/>
-    <tableColumn id="1" name="Keywert" dataDxfId="4"/>
-    <tableColumn id="3" name="Schreibungsvarianten Baernreither" dataDxfId="3"/>
-    <tableColumn id="4" name="Bezeichnung" dataDxfId="2"/>
-    <tableColumn id="2" name="GeoNames" dataDxfId="1"/>
-    <tableColumn id="6" name="Spalte1" dataDxfId="0"/>
+    <tableColumn id="5" name="aktuelle Schreibung" dataDxfId="7"/>
+    <tableColumn id="1" name="Keywert" dataDxfId="6"/>
+    <tableColumn id="3" name="Schreibungsvarianten Baernreither" dataDxfId="5"/>
+    <tableColumn id="4" name="Bezeichnung" dataDxfId="4"/>
+    <tableColumn id="2" name="GeoNames" dataDxfId="3"/>
+    <tableColumn id="6" name="Spalte1" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1443,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="134" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1460,10 +1493,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
@@ -1475,873 +1508,879 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>308</v>
+      </c>
       <c r="B3" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>37</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>98</v>
+        <v>308</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>211</v>
+        <v>309</v>
       </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>211</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="D4" s="4" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>0</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>203</v>
+        <v>88</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D7" s="4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="B8" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>216</v>
+      </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
+      <c r="D8" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>51</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>221</v>
-      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>81</v>
+        <v>205</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>123</v>
+        <v>194</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>255</v>
+        <v>40</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>196</v>
+        <v>119</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>124</v>
+        <v>192</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>8</v>
+        <v>303</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>197</v>
+        <v>126</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>230</v>
+    <row r="17" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="F19" s="4"/>
+    <row r="18" spans="1:6" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>266</v>
+    <row r="22" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>234</v>
+    <row r="23" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>261</v>
       </c>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
+      <c r="A24" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="B24" s="4" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>199</v>
+        <v>103</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>96</v>
-      </c>
+      <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
+    <row r="27" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="B27" s="4" t="s">
-        <v>18</v>
+        <v>300</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4" t="s">
-        <v>198</v>
+        <v>95</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
-        <v>103</v>
+        <v>194</v>
       </c>
       <c r="E31" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="F31" s="4"/>
-    </row>
-    <row r="32" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4" t="s">
-        <v>246</v>
-      </c>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="16" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>280</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>16</v>
+        <v>272</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D39" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="F40" s="4"/>
-    </row>
-    <row r="41" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
+        <v>128</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="B41" s="4" t="s">
-        <v>263</v>
+        <v>46</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E41" s="4"/>
+        <v>130</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>283</v>
+      </c>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>109</v>
-      </c>
+    <row r="42" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
       <c r="B42" s="4" t="s">
-        <v>40</v>
+        <v>258</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>287</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
+    <row r="44" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="B44" s="4" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>113</v>
-      </c>
+    <row r="45" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
       <c r="B45" s="4" t="s">
-        <v>259</v>
+        <v>37</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E49" s="4"/>
+        <v>133</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>246</v>
+      </c>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A50" s="4"/>
+    <row r="50" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="B50" s="4" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>268</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="E50" s="4"/>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
-        <v>141</v>
-      </c>
+    <row r="51" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E51" s="4"/>
+        <v>136</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>263</v>
+      </c>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>290</v>
+        <v>35</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>291</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A53" s="4"/>
+    <row r="53" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="B53" s="4" t="s">
-        <v>57</v>
+        <v>285</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
-        <v>289</v>
+        <v>53</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="E54" s="4"/>
+        <v>140</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>289</v>
+      </c>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4" t="s">
-        <v>61</v>
+        <v>284</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>295</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="E55" s="4"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
-        <v>146</v>
-      </c>
+    <row r="56" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
       <c r="B56" s="4" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>267</v>
+        <v>290</v>
       </c>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>258</v>
+        <v>65</v>
       </c>
       <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
+      <c r="D57" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="E57" s="4" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C58" s="4"/>
-      <c r="D58" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="E58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4" t="s">
+        <v>277</v>
+      </c>
       <c r="F58" s="4"/>
     </row>
     <row r="59" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A59" s="4"/>
+      <c r="A59" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="B59" s="4" t="s">
-        <v>54</v>
+        <v>251</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4" t="s">
@@ -2351,505 +2390,533 @@
       <c r="F59" s="4"/>
     </row>
     <row r="60" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
-        <v>149</v>
-      </c>
+      <c r="A60" s="4"/>
       <c r="B60" s="4" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>293</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="E60" s="4"/>
       <c r="F60" s="4"/>
     </row>
     <row r="61" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="F61" s="4"/>
     </row>
     <row r="62" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="F62" s="4"/>
     </row>
     <row r="63" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E63" s="4"/>
+        <v>149</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>269</v>
+      </c>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="4"/>
+    <row r="64" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="B64" s="4" t="s">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>275</v>
+        <v>305</v>
       </c>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
-        <v>7</v>
-      </c>
+    <row r="65" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
       <c r="B65" s="4" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F65" s="4"/>
     </row>
     <row r="66" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A66" s="4"/>
+      <c r="A66" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="B66" s="4" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E66" s="4"/>
+        <v>160</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>264</v>
+      </c>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
-        <v>160</v>
-      </c>
+    <row r="67" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
       <c r="B67" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>1</v>
+        <v>295</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>257</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="E68" s="4"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="4"/>
+    <row r="69" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>155</v>
+      </c>
       <c r="B69" s="4" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E69" s="4"/>
+        <v>158</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>252</v>
+      </c>
       <c r="F69" s="4"/>
     </row>
     <row r="70" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="4" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="E70" s="4"/>
+        <v>161</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>298</v>
+      </c>
       <c r="F70" s="4"/>
     </row>
-    <row r="71" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
-        <v>152</v>
-      </c>
+    <row r="71" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="4"/>
       <c r="B71" s="4" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="4" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>272</v>
+        <v>294</v>
       </c>
       <c r="F71" s="4"/>
     </row>
     <row r="72" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A73" s="4"/>
+    <row r="73" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="B73" s="4" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="4" t="s">
-        <v>168</v>
+        <v>112</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>271</v>
       </c>
       <c r="F73" s="4"/>
     </row>
-    <row r="74" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="B74" s="4" t="s">
-        <v>298</v>
+        <v>9</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>297</v>
+        <v>266</v>
       </c>
       <c r="F74" s="4"/>
     </row>
-    <row r="75" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
-        <v>29</v>
-      </c>
+    <row r="75" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="4"/>
       <c r="B75" s="4" t="s">
-        <v>29</v>
+        <v>293</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="F75" s="4"/>
     </row>
     <row r="76" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>171</v>
+        <v>26</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C76" s="4"/>
       <c r="D76" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="F76" s="4"/>
     </row>
     <row r="77" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C77" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="D77" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="E77" s="4"/>
+        <v>168</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>256</v>
+      </c>
       <c r="F77" s="4"/>
     </row>
     <row r="78" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
     </row>
     <row r="79" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="C79" s="4"/>
       <c r="D79" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E79" s="4"/>
+        <v>172</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>302</v>
+      </c>
       <c r="F79" s="4"/>
     </row>
     <row r="80" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A80" s="4"/>
+      <c r="A80" s="4" t="s">
+        <v>173</v>
+      </c>
       <c r="B80" s="4" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>284</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="E80" s="4"/>
       <c r="F80" s="4"/>
     </row>
     <row r="81" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
-        <v>180</v>
-      </c>
+      <c r="A81" s="4"/>
       <c r="B81" s="4" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4" t="s">
-        <v>124</v>
+        <v>187</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>252</v>
+        <v>279</v>
       </c>
       <c r="F81" s="4"/>
     </row>
     <row r="82" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A82" s="4"/>
+      <c r="A82" s="4" t="s">
+        <v>176</v>
+      </c>
       <c r="B82" s="4" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="C82" s="4"/>
       <c r="D82" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="E82" s="4"/>
+        <v>120</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>247</v>
+      </c>
       <c r="F82" s="4"/>
     </row>
-    <row r="83" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
-        <v>24</v>
-      </c>
+    <row r="83" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A83" s="4"/>
       <c r="B83" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="E83" s="4"/>
+        <v>178</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>297</v>
+      </c>
       <c r="F83" s="4"/>
     </row>
-    <row r="84" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>181</v>
+        <v>23</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="E84" s="4"/>
-      <c r="F84" s="6"/>
-    </row>
-    <row r="85" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F84" s="4"/>
+    </row>
+    <row r="85" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="C85" s="4"/>
       <c r="D85" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="F85" s="4"/>
+        <v>301</v>
+      </c>
+      <c r="F85" s="6"/>
     </row>
     <row r="86" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A86" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D86" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="E86" s="6"/>
+      <c r="A86" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>278</v>
+      </c>
       <c r="F86" s="4"/>
     </row>
     <row r="87" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4" t="s">
+      <c r="A87" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E87" s="6"/>
+      <c r="F87" s="4"/>
+    </row>
+    <row r="88" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="F87" s="4"/>
-    </row>
-    <row r="88" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>262</v>
       </c>
       <c r="C88" s="4"/>
       <c r="D88" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E88" s="4"/>
+        <v>181</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>276</v>
+      </c>
       <c r="F88" s="4"/>
     </row>
-    <row r="89" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>2</v>
+        <v>182</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>2</v>
+        <v>257</v>
       </c>
       <c r="C89" s="4"/>
-      <c r="D89" s="4"/>
+      <c r="D89" s="4" t="s">
+        <v>203</v>
+      </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C90" s="7"/>
-      <c r="D90" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>296</v>
-      </c>
+    <row r="90" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
       <c r="F90" s="4"/>
     </row>
-    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>20</v>
+        <v>183</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="E91" s="7"/>
+        <v>184</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>291</v>
+      </c>
       <c r="F91" s="4"/>
+    </row>
+    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A92" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="F92" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId1"/>
     <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E10" r:id="rId7"/>
-    <hyperlink ref="E11" r:id="rId8"/>
-    <hyperlink ref="E12" r:id="rId9"/>
-    <hyperlink ref="E13" r:id="rId10"/>
-    <hyperlink ref="E14" r:id="rId11"/>
-    <hyperlink ref="E15" r:id="rId12"/>
-    <hyperlink ref="E16" r:id="rId13"/>
-    <hyperlink ref="E18" r:id="rId14"/>
-    <hyperlink ref="E17" r:id="rId15"/>
-    <hyperlink ref="E19" r:id="rId16"/>
-    <hyperlink ref="E20" r:id="rId17"/>
-    <hyperlink ref="E21" r:id="rId18"/>
-    <hyperlink ref="E23" r:id="rId19"/>
-    <hyperlink ref="E24" r:id="rId20"/>
-    <hyperlink ref="E25" r:id="rId21"/>
-    <hyperlink ref="E26" r:id="rId22"/>
-    <hyperlink ref="E27" r:id="rId23"/>
-    <hyperlink ref="E28" r:id="rId24"/>
-    <hyperlink ref="E29" r:id="rId25"/>
-    <hyperlink ref="E9" r:id="rId26"/>
-    <hyperlink ref="E30" r:id="rId27"/>
-    <hyperlink ref="E31" r:id="rId28"/>
-    <hyperlink ref="E34" r:id="rId29"/>
-    <hyperlink ref="E35" r:id="rId30"/>
-    <hyperlink ref="E36" r:id="rId31"/>
-    <hyperlink ref="E39" r:id="rId32"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E6" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="E11" r:id="rId7"/>
+    <hyperlink ref="E12" r:id="rId8"/>
+    <hyperlink ref="E13" r:id="rId9"/>
+    <hyperlink ref="E14" r:id="rId10"/>
+    <hyperlink ref="E15" r:id="rId11"/>
+    <hyperlink ref="E16" r:id="rId12"/>
+    <hyperlink ref="E17" r:id="rId13"/>
+    <hyperlink ref="E19" r:id="rId14"/>
+    <hyperlink ref="E18" r:id="rId15"/>
+    <hyperlink ref="E20" r:id="rId16"/>
+    <hyperlink ref="E21" r:id="rId17"/>
+    <hyperlink ref="E22" r:id="rId18"/>
+    <hyperlink ref="E24" r:id="rId19"/>
+    <hyperlink ref="E25" r:id="rId20"/>
+    <hyperlink ref="E26" r:id="rId21"/>
+    <hyperlink ref="E27" r:id="rId22"/>
+    <hyperlink ref="E28" r:id="rId23"/>
+    <hyperlink ref="E29" r:id="rId24"/>
+    <hyperlink ref="E30" r:id="rId25"/>
+    <hyperlink ref="E10" r:id="rId26"/>
+    <hyperlink ref="E31" r:id="rId27"/>
+    <hyperlink ref="E35" r:id="rId28"/>
+    <hyperlink ref="E36" r:id="rId29"/>
+    <hyperlink ref="E37" r:id="rId30"/>
+    <hyperlink ref="E40" r:id="rId31"/>
+    <hyperlink ref="E32" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>

</xml_diff>